<commit_message>
Left join to add the data of income
</commit_message>
<xml_diff>
--- a/data /income_2015.xlsx
+++ b/data /income_2015.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qinyaowu/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/qinyaowu/Desktop/P8105_final_project/data /"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -752,7 +752,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -879,15 +879,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color rgb="FFAAC1D9"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFAAC1D9"/>
       </left>
@@ -965,7 +956,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -989,7 +980,7 @@
     <xf numFmtId="0" fontId="6" fillId="36" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -998,22 +989,19 @@
     <xf numFmtId="0" fontId="5" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="35" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1363,8 +1351,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BN59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="179" workbookViewId="0">
-      <selection activeCell="B56" sqref="B56"/>
+    <sheetView tabSelected="1" zoomScale="179" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1376,82 +1364,78 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:66" s="2" customFormat="1" ht="3" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="12"/>
-      <c r="L1" s="12"/>
-      <c r="M1" s="12"/>
-      <c r="N1" s="12"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="12"/>
-      <c r="R1" s="12"/>
-      <c r="S1" s="12"/>
-      <c r="T1" s="12"/>
-      <c r="U1" s="12"/>
-      <c r="V1" s="12"/>
-      <c r="W1" s="12"/>
-      <c r="X1" s="12"/>
-      <c r="Y1" s="12"/>
-      <c r="Z1" s="12"/>
-      <c r="AA1" s="12"/>
-      <c r="AB1" s="12"/>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="12"/>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="12"/>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="12"/>
-      <c r="BL1" s="12"/>
-      <c r="BM1" s="12"/>
-      <c r="BN1" s="12"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="14"/>
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="14"/>
+      <c r="BG1" s="14"/>
+      <c r="BH1" s="14"/>
+      <c r="BI1" s="14"/>
+      <c r="BJ1" s="14"/>
+      <c r="BK1" s="14"/>
+      <c r="BL1" s="14"/>
+      <c r="BM1" s="14"/>
+      <c r="BN1" s="14"/>
     </row>
     <row r="2" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="17" t="s">
-        <v>60</v>
-      </c>
+      <c r="A2" s="12"/>
+      <c r="B2" s="13"/>
       <c r="C2" s="15" t="s">
         <v>3</v>
       </c>
@@ -1516,8 +1500,12 @@
       <c r="BJ2" s="7"/>
     </row>
     <row r="3" spans="1:66" ht="24" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="16"/>
+      <c r="A3" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>60</v>
+      </c>
       <c r="C3" s="9" t="s">
         <v>5</v>
       </c>
@@ -5532,11 +5520,9 @@
     </row>
     <row r="59" spans="1:66" ht="13" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="2">
     <mergeCell ref="A1:BN1"/>
-    <mergeCell ref="A2:A3"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B2:B3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A58" r:id="rId1" display="//www2.census.gov/programs-surveys/cps/techdocs/cpsmar16.pdf"/>

</xml_diff>